<commit_message>
Added something in sheets
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4131" uniqueCount="866">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4130" uniqueCount="865">
   <si>
     <t>COLORHISTOGRAM</t>
   </si>
@@ -2622,9 +2622,6 @@
   </si>
   <si>
     <t>precision</t>
-  </si>
-  <si>
-    <t>recall</t>
   </si>
   <si>
     <t>Average precision</t>
@@ -43692,7 +43689,7 @@
   <dimension ref="A1:AO13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -44766,14 +44763,9 @@
         <v>0.36363636363636365</v>
       </c>
     </row>
-    <row r="8" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>864</v>
-      </c>
-    </row>
     <row r="12" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
       <c r="B12" t="s">
         <v>0</v>

</xml_diff>

<commit_message>
Added chart in results excel
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -9,13 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15460" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15460" tabRatio="500" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="results" sheetId="1" r:id="rId1"/>
     <sheet name="concat" sheetId="3" r:id="rId2"/>
     <sheet name="transpose" sheetId="4" r:id="rId3"/>
-    <sheet name="Sheet1" sheetId="2" r:id="rId4"/>
+    <sheet name="Summary" sheetId="2" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5161" uniqueCount="869">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5166" uniqueCount="874">
   <si>
     <t>COLORHISTOGRAM</t>
   </si>
@@ -2637,13 +2638,28 @@
   </si>
   <si>
     <t>942.jpg</t>
+  </si>
+  <si>
+    <t>Color Histogram</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CH with Perceptual Similarity incorporated </t>
+  </si>
+  <si>
+    <t>Histogram Refinement with Color Coherence</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CH with Centering Refinement </t>
+  </si>
+  <si>
+    <t>CH with Centering Refinement and Color Coherence</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -2666,6 +2682,11 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="TwCenMT"/>
     </font>
   </fonts>
   <fills count="2">
@@ -2692,8 +2713,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -2710,6 +2733,919 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-PH"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx2"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Method Precision</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx2"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:gradFill rotWithShape="1">
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:schemeClr val="accent1">
+                    <a:satMod val="103000"/>
+                    <a:lumMod val="102000"/>
+                    <a:tint val="94000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="50000">
+                  <a:schemeClr val="accent1">
+                    <a:satMod val="110000"/>
+                    <a:lumMod val="100000"/>
+                    <a:shade val="100000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:schemeClr val="accent1">
+                    <a:lumMod val="99000"/>
+                    <a:satMod val="120000"/>
+                    <a:shade val="78000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="5400000" scaled="0"/>
+            </a:gradFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx2"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="inEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="tx2">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$1:$E$1</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>Color Histogram</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>CH with Perceptual Similarity incorporated </c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Histogram Refinement with Color Coherence</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>CH with Centering Refinement </c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>CH with Centering Refinement and Color Coherence</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$A$2:$E$2</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.360606060606061</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.45959595959596</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.494949494949495</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.506060606060606</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.497979797979798</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="inEnd"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="100"/>
+        <c:overlap val="-24"/>
+        <c:axId val="-442162048"/>
+        <c:axId val="-406896560"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="-442162048"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx2">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx2"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-406896560"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-406896560"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx2">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx2"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-442162048"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx2">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="207">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk2">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="2"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="2"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="2"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="31750" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="2"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="12700">
+        <a:solidFill>
+          <a:schemeClr val="lt2"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="2"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" kern="1200"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>508000</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>558800</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -53825,8 +54761,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AY13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -55206,4 +56142,61 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="21.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="35.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="37.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="42.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>869</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>870</v>
+      </c>
+      <c r="C1" t="s">
+        <v>871</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>872</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>873</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="2">
+        <v>0.3606060606060606</v>
+      </c>
+      <c r="B2" s="2">
+        <v>0.45959595959595961</v>
+      </c>
+      <c r="C2" s="2">
+        <v>0.49494949494949492</v>
+      </c>
+      <c r="D2" s="2">
+        <v>0.5060606060606061</v>
+      </c>
+      <c r="E2" s="2">
+        <v>0.49797979797979791</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added top results per subclass
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15460" tabRatio="500" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15460" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="results" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5166" uniqueCount="874">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5235" uniqueCount="877">
   <si>
     <t>COLORHISTOGRAM</t>
   </si>
@@ -2653,6 +2653,15 @@
   </si>
   <si>
     <t>CH with Centering Refinement and Color Coherence</t>
+  </si>
+  <si>
+    <t>TOP Methods</t>
+  </si>
+  <si>
+    <t>Subclass</t>
+  </si>
+  <si>
+    <t>Method</t>
   </si>
 </sst>
 </file>
@@ -2725,7 +2734,18 @@
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -2956,11 +2976,11 @@
         </c:dLbls>
         <c:gapWidth val="100"/>
         <c:overlap val="-24"/>
-        <c:axId val="-442162048"/>
-        <c:axId val="-406896560"/>
+        <c:axId val="-1614211600"/>
+        <c:axId val="-1610925936"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-442162048"/>
+        <c:axId val="-1614211600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3000,7 +3020,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-406896560"/>
+        <c:crossAx val="-1610925936"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3008,7 +3028,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-406896560"/>
+        <c:axId val="-1610925936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3055,7 +3075,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-442162048"/>
+        <c:crossAx val="-1614211600"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -54759,13 +54779,16 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AY13"/>
+  <dimension ref="A1:AY43"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="B43" sqref="B43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="17.5" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:51" x14ac:dyDescent="0.2">
       <c r="B1">
@@ -56138,7 +56161,1302 @@
         <v>0.49797979797979791</v>
       </c>
     </row>
+    <row r="15" spans="1:51" x14ac:dyDescent="0.2">
+      <c r="B15">
+        <v>0</v>
+      </c>
+      <c r="C15">
+        <v>0</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
+      </c>
+      <c r="F15">
+        <v>0</v>
+      </c>
+      <c r="G15">
+        <v>1</v>
+      </c>
+      <c r="H15">
+        <v>1</v>
+      </c>
+      <c r="I15">
+        <v>1</v>
+      </c>
+      <c r="J15">
+        <v>1</v>
+      </c>
+      <c r="K15">
+        <v>1</v>
+      </c>
+      <c r="L15">
+        <v>2</v>
+      </c>
+      <c r="M15">
+        <v>2</v>
+      </c>
+      <c r="N15">
+        <v>2</v>
+      </c>
+      <c r="O15">
+        <v>2</v>
+      </c>
+      <c r="P15">
+        <v>2</v>
+      </c>
+      <c r="Q15">
+        <v>3</v>
+      </c>
+      <c r="R15">
+        <v>3</v>
+      </c>
+      <c r="S15">
+        <v>3</v>
+      </c>
+      <c r="T15">
+        <v>3</v>
+      </c>
+      <c r="U15">
+        <v>3</v>
+      </c>
+      <c r="V15">
+        <v>4</v>
+      </c>
+      <c r="W15">
+        <v>4</v>
+      </c>
+      <c r="X15">
+        <v>4</v>
+      </c>
+      <c r="Y15">
+        <v>4</v>
+      </c>
+      <c r="Z15">
+        <v>4</v>
+      </c>
+      <c r="AA15">
+        <v>5</v>
+      </c>
+      <c r="AB15">
+        <v>5</v>
+      </c>
+      <c r="AC15">
+        <v>5</v>
+      </c>
+      <c r="AD15">
+        <v>5</v>
+      </c>
+      <c r="AE15">
+        <v>5</v>
+      </c>
+      <c r="AF15">
+        <v>6</v>
+      </c>
+      <c r="AG15">
+        <v>6</v>
+      </c>
+      <c r="AH15">
+        <v>6</v>
+      </c>
+      <c r="AI15">
+        <v>6</v>
+      </c>
+      <c r="AJ15">
+        <v>6</v>
+      </c>
+      <c r="AK15">
+        <v>7</v>
+      </c>
+      <c r="AL15">
+        <v>7</v>
+      </c>
+      <c r="AM15">
+        <v>7</v>
+      </c>
+      <c r="AN15">
+        <v>7</v>
+      </c>
+      <c r="AO15">
+        <v>7</v>
+      </c>
+      <c r="AP15">
+        <v>8</v>
+      </c>
+      <c r="AQ15">
+        <v>8</v>
+      </c>
+      <c r="AR15">
+        <v>8</v>
+      </c>
+      <c r="AS15">
+        <v>8</v>
+      </c>
+      <c r="AT15">
+        <v>8</v>
+      </c>
+      <c r="AU15">
+        <v>9</v>
+      </c>
+      <c r="AV15">
+        <v>9</v>
+      </c>
+      <c r="AW15">
+        <v>9</v>
+      </c>
+      <c r="AX15">
+        <v>9</v>
+      </c>
+      <c r="AY15">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:51" x14ac:dyDescent="0.2">
+      <c r="B16" t="s">
+        <v>0</v>
+      </c>
+      <c r="C16" t="s">
+        <v>100</v>
+      </c>
+      <c r="D16" t="s">
+        <v>128</v>
+      </c>
+      <c r="E16" t="s">
+        <v>144</v>
+      </c>
+      <c r="F16" t="s">
+        <v>865</v>
+      </c>
+      <c r="G16" t="s">
+        <v>0</v>
+      </c>
+      <c r="H16" t="s">
+        <v>100</v>
+      </c>
+      <c r="I16" t="s">
+        <v>128</v>
+      </c>
+      <c r="J16" t="s">
+        <v>144</v>
+      </c>
+      <c r="K16" t="s">
+        <v>865</v>
+      </c>
+      <c r="L16" t="s">
+        <v>0</v>
+      </c>
+      <c r="M16" t="s">
+        <v>100</v>
+      </c>
+      <c r="N16" t="s">
+        <v>128</v>
+      </c>
+      <c r="O16" t="s">
+        <v>144</v>
+      </c>
+      <c r="P16" t="s">
+        <v>865</v>
+      </c>
+      <c r="Q16" t="s">
+        <v>0</v>
+      </c>
+      <c r="R16" t="s">
+        <v>100</v>
+      </c>
+      <c r="S16" t="s">
+        <v>128</v>
+      </c>
+      <c r="T16" t="s">
+        <v>144</v>
+      </c>
+      <c r="U16" t="s">
+        <v>865</v>
+      </c>
+      <c r="V16" t="s">
+        <v>0</v>
+      </c>
+      <c r="W16" t="s">
+        <v>100</v>
+      </c>
+      <c r="X16" t="s">
+        <v>128</v>
+      </c>
+      <c r="Y16" t="s">
+        <v>144</v>
+      </c>
+      <c r="Z16" t="s">
+        <v>865</v>
+      </c>
+      <c r="AA16" t="s">
+        <v>0</v>
+      </c>
+      <c r="AB16" t="s">
+        <v>100</v>
+      </c>
+      <c r="AC16" t="s">
+        <v>128</v>
+      </c>
+      <c r="AD16" t="s">
+        <v>144</v>
+      </c>
+      <c r="AE16" t="s">
+        <v>865</v>
+      </c>
+      <c r="AF16" t="s">
+        <v>0</v>
+      </c>
+      <c r="AG16" t="s">
+        <v>100</v>
+      </c>
+      <c r="AH16" t="s">
+        <v>128</v>
+      </c>
+      <c r="AI16" t="s">
+        <v>144</v>
+      </c>
+      <c r="AJ16" t="s">
+        <v>865</v>
+      </c>
+      <c r="AK16" t="s">
+        <v>0</v>
+      </c>
+      <c r="AL16" t="s">
+        <v>100</v>
+      </c>
+      <c r="AM16" t="s">
+        <v>128</v>
+      </c>
+      <c r="AN16" t="s">
+        <v>144</v>
+      </c>
+      <c r="AO16" t="s">
+        <v>865</v>
+      </c>
+      <c r="AP16" t="s">
+        <v>0</v>
+      </c>
+      <c r="AQ16" t="s">
+        <v>100</v>
+      </c>
+      <c r="AR16" t="s">
+        <v>128</v>
+      </c>
+      <c r="AS16" t="s">
+        <v>144</v>
+      </c>
+      <c r="AT16" t="s">
+        <v>865</v>
+      </c>
+      <c r="AU16" t="s">
+        <v>0</v>
+      </c>
+      <c r="AV16" t="s">
+        <v>100</v>
+      </c>
+      <c r="AW16" t="s">
+        <v>128</v>
+      </c>
+      <c r="AX16" t="s">
+        <v>144</v>
+      </c>
+      <c r="AY16" t="s">
+        <v>865</v>
+      </c>
+    </row>
+    <row r="17" spans="1:51" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>859</v>
+      </c>
+      <c r="B17">
+        <v>32</v>
+      </c>
+      <c r="C17">
+        <v>47</v>
+      </c>
+      <c r="D17">
+        <v>43</v>
+      </c>
+      <c r="E17">
+        <v>48</v>
+      </c>
+      <c r="F17">
+        <v>45</v>
+      </c>
+      <c r="G17">
+        <v>30</v>
+      </c>
+      <c r="H17">
+        <v>31</v>
+      </c>
+      <c r="I17">
+        <v>28</v>
+      </c>
+      <c r="J17">
+        <v>36</v>
+      </c>
+      <c r="K17">
+        <v>38</v>
+      </c>
+      <c r="L17">
+        <v>30</v>
+      </c>
+      <c r="M17">
+        <v>43</v>
+      </c>
+      <c r="N17">
+        <v>32</v>
+      </c>
+      <c r="O17">
+        <v>48</v>
+      </c>
+      <c r="P17">
+        <v>47</v>
+      </c>
+      <c r="Q17">
+        <v>50</v>
+      </c>
+      <c r="R17">
+        <v>36</v>
+      </c>
+      <c r="S17">
+        <v>39</v>
+      </c>
+      <c r="T17">
+        <v>33</v>
+      </c>
+      <c r="U17">
+        <v>29</v>
+      </c>
+      <c r="V17">
+        <v>28</v>
+      </c>
+      <c r="W17">
+        <v>96</v>
+      </c>
+      <c r="X17">
+        <v>96</v>
+      </c>
+      <c r="Y17">
+        <v>97</v>
+      </c>
+      <c r="Z17">
+        <v>97</v>
+      </c>
+      <c r="AA17">
+        <v>32</v>
+      </c>
+      <c r="AB17">
+        <v>49</v>
+      </c>
+      <c r="AC17">
+        <v>45</v>
+      </c>
+      <c r="AD17">
+        <v>48</v>
+      </c>
+      <c r="AE17">
+        <v>48</v>
+      </c>
+      <c r="AF17">
+        <v>29</v>
+      </c>
+      <c r="AG17">
+        <v>46</v>
+      </c>
+      <c r="AH17">
+        <v>35</v>
+      </c>
+      <c r="AI17">
+        <v>41</v>
+      </c>
+      <c r="AJ17">
+        <v>44</v>
+      </c>
+      <c r="AK17">
+        <v>59</v>
+      </c>
+      <c r="AL17">
+        <v>76</v>
+      </c>
+      <c r="AM17">
+        <v>67</v>
+      </c>
+      <c r="AN17">
+        <v>70</v>
+      </c>
+      <c r="AO17">
+        <v>74</v>
+      </c>
+      <c r="AP17">
+        <v>25</v>
+      </c>
+      <c r="AQ17">
+        <v>38</v>
+      </c>
+      <c r="AR17">
+        <v>30</v>
+      </c>
+      <c r="AS17">
+        <v>33</v>
+      </c>
+      <c r="AT17">
+        <v>34</v>
+      </c>
+      <c r="AU17">
+        <v>42</v>
+      </c>
+      <c r="AV17">
+        <v>39</v>
+      </c>
+      <c r="AW17">
+        <v>40</v>
+      </c>
+      <c r="AX17">
+        <v>36</v>
+      </c>
+      <c r="AY17">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="18" spans="1:51" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>860</v>
+      </c>
+      <c r="B18">
+        <v>67</v>
+      </c>
+      <c r="C18">
+        <v>52</v>
+      </c>
+      <c r="D18">
+        <v>56</v>
+      </c>
+      <c r="E18">
+        <v>51</v>
+      </c>
+      <c r="F18">
+        <v>54</v>
+      </c>
+      <c r="G18">
+        <v>69</v>
+      </c>
+      <c r="H18">
+        <v>68</v>
+      </c>
+      <c r="I18">
+        <v>71</v>
+      </c>
+      <c r="J18">
+        <v>63</v>
+      </c>
+      <c r="K18">
+        <v>61</v>
+      </c>
+      <c r="L18">
+        <v>69</v>
+      </c>
+      <c r="M18">
+        <v>56</v>
+      </c>
+      <c r="N18">
+        <v>67</v>
+      </c>
+      <c r="O18">
+        <v>51</v>
+      </c>
+      <c r="P18">
+        <v>52</v>
+      </c>
+      <c r="Q18">
+        <v>49</v>
+      </c>
+      <c r="R18">
+        <v>63</v>
+      </c>
+      <c r="S18">
+        <v>60</v>
+      </c>
+      <c r="T18">
+        <v>66</v>
+      </c>
+      <c r="U18">
+        <v>70</v>
+      </c>
+      <c r="V18">
+        <v>71</v>
+      </c>
+      <c r="W18">
+        <v>3</v>
+      </c>
+      <c r="X18">
+        <v>3</v>
+      </c>
+      <c r="Y18">
+        <v>2</v>
+      </c>
+      <c r="Z18">
+        <v>2</v>
+      </c>
+      <c r="AA18">
+        <v>67</v>
+      </c>
+      <c r="AB18">
+        <v>50</v>
+      </c>
+      <c r="AC18">
+        <v>54</v>
+      </c>
+      <c r="AD18">
+        <v>51</v>
+      </c>
+      <c r="AE18">
+        <v>51</v>
+      </c>
+      <c r="AF18">
+        <v>70</v>
+      </c>
+      <c r="AG18">
+        <v>53</v>
+      </c>
+      <c r="AH18">
+        <v>64</v>
+      </c>
+      <c r="AI18">
+        <v>58</v>
+      </c>
+      <c r="AJ18">
+        <v>55</v>
+      </c>
+      <c r="AK18">
+        <v>40</v>
+      </c>
+      <c r="AL18">
+        <v>23</v>
+      </c>
+      <c r="AM18">
+        <v>32</v>
+      </c>
+      <c r="AN18">
+        <v>29</v>
+      </c>
+      <c r="AO18">
+        <v>25</v>
+      </c>
+      <c r="AP18">
+        <v>74</v>
+      </c>
+      <c r="AQ18">
+        <v>61</v>
+      </c>
+      <c r="AR18">
+        <v>69</v>
+      </c>
+      <c r="AS18">
+        <v>66</v>
+      </c>
+      <c r="AT18">
+        <v>65</v>
+      </c>
+      <c r="AU18">
+        <v>57</v>
+      </c>
+      <c r="AV18">
+        <v>60</v>
+      </c>
+      <c r="AW18">
+        <v>59</v>
+      </c>
+      <c r="AX18">
+        <v>63</v>
+      </c>
+      <c r="AY18">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="19" spans="1:51" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>861</v>
+      </c>
+      <c r="B19">
+        <v>67</v>
+      </c>
+      <c r="C19">
+        <v>52</v>
+      </c>
+      <c r="D19">
+        <v>56</v>
+      </c>
+      <c r="E19">
+        <v>51</v>
+      </c>
+      <c r="F19">
+        <v>54</v>
+      </c>
+      <c r="G19">
+        <v>69</v>
+      </c>
+      <c r="H19">
+        <v>68</v>
+      </c>
+      <c r="I19">
+        <v>71</v>
+      </c>
+      <c r="J19">
+        <v>63</v>
+      </c>
+      <c r="K19">
+        <v>61</v>
+      </c>
+      <c r="L19">
+        <v>69</v>
+      </c>
+      <c r="M19">
+        <v>56</v>
+      </c>
+      <c r="N19">
+        <v>67</v>
+      </c>
+      <c r="O19">
+        <v>51</v>
+      </c>
+      <c r="P19">
+        <v>52</v>
+      </c>
+      <c r="Q19">
+        <v>49</v>
+      </c>
+      <c r="R19">
+        <v>63</v>
+      </c>
+      <c r="S19">
+        <v>60</v>
+      </c>
+      <c r="T19">
+        <v>66</v>
+      </c>
+      <c r="U19">
+        <v>70</v>
+      </c>
+      <c r="V19">
+        <v>71</v>
+      </c>
+      <c r="W19">
+        <v>3</v>
+      </c>
+      <c r="X19">
+        <v>3</v>
+      </c>
+      <c r="Y19">
+        <v>2</v>
+      </c>
+      <c r="Z19">
+        <v>2</v>
+      </c>
+      <c r="AA19">
+        <v>67</v>
+      </c>
+      <c r="AB19">
+        <v>50</v>
+      </c>
+      <c r="AC19">
+        <v>54</v>
+      </c>
+      <c r="AD19">
+        <v>51</v>
+      </c>
+      <c r="AE19">
+        <v>51</v>
+      </c>
+      <c r="AF19">
+        <v>70</v>
+      </c>
+      <c r="AG19">
+        <v>53</v>
+      </c>
+      <c r="AH19">
+        <v>64</v>
+      </c>
+      <c r="AI19">
+        <v>58</v>
+      </c>
+      <c r="AJ19">
+        <v>55</v>
+      </c>
+      <c r="AK19">
+        <v>40</v>
+      </c>
+      <c r="AL19">
+        <v>23</v>
+      </c>
+      <c r="AM19">
+        <v>32</v>
+      </c>
+      <c r="AN19">
+        <v>29</v>
+      </c>
+      <c r="AO19">
+        <v>25</v>
+      </c>
+      <c r="AP19">
+        <v>74</v>
+      </c>
+      <c r="AQ19">
+        <v>61</v>
+      </c>
+      <c r="AR19">
+        <v>69</v>
+      </c>
+      <c r="AS19">
+        <v>66</v>
+      </c>
+      <c r="AT19">
+        <v>65</v>
+      </c>
+      <c r="AU19">
+        <v>57</v>
+      </c>
+      <c r="AV19">
+        <v>60</v>
+      </c>
+      <c r="AW19">
+        <v>59</v>
+      </c>
+      <c r="AX19">
+        <v>63</v>
+      </c>
+      <c r="AY19">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="20" spans="1:51" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>862</v>
+      </c>
+      <c r="B20">
+        <v>833</v>
+      </c>
+      <c r="C20">
+        <v>848</v>
+      </c>
+      <c r="D20">
+        <v>844</v>
+      </c>
+      <c r="E20">
+        <v>849</v>
+      </c>
+      <c r="F20">
+        <v>846</v>
+      </c>
+      <c r="G20">
+        <v>831</v>
+      </c>
+      <c r="H20">
+        <v>832</v>
+      </c>
+      <c r="I20">
+        <v>829</v>
+      </c>
+      <c r="J20">
+        <v>837</v>
+      </c>
+      <c r="K20">
+        <v>839</v>
+      </c>
+      <c r="L20">
+        <v>831</v>
+      </c>
+      <c r="M20">
+        <v>844</v>
+      </c>
+      <c r="N20">
+        <v>833</v>
+      </c>
+      <c r="O20">
+        <v>849</v>
+      </c>
+      <c r="P20">
+        <v>848</v>
+      </c>
+      <c r="Q20">
+        <v>851</v>
+      </c>
+      <c r="R20">
+        <v>837</v>
+      </c>
+      <c r="S20">
+        <v>840</v>
+      </c>
+      <c r="T20">
+        <v>834</v>
+      </c>
+      <c r="U20">
+        <v>830</v>
+      </c>
+      <c r="V20">
+        <v>829</v>
+      </c>
+      <c r="W20">
+        <v>897</v>
+      </c>
+      <c r="X20">
+        <v>897</v>
+      </c>
+      <c r="Y20">
+        <v>898</v>
+      </c>
+      <c r="Z20">
+        <v>898</v>
+      </c>
+      <c r="AA20">
+        <v>833</v>
+      </c>
+      <c r="AB20">
+        <v>850</v>
+      </c>
+      <c r="AC20">
+        <v>846</v>
+      </c>
+      <c r="AD20">
+        <v>849</v>
+      </c>
+      <c r="AE20">
+        <v>849</v>
+      </c>
+      <c r="AF20">
+        <v>830</v>
+      </c>
+      <c r="AG20">
+        <v>847</v>
+      </c>
+      <c r="AH20">
+        <v>836</v>
+      </c>
+      <c r="AI20">
+        <v>842</v>
+      </c>
+      <c r="AJ20">
+        <v>845</v>
+      </c>
+      <c r="AK20">
+        <v>860</v>
+      </c>
+      <c r="AL20">
+        <v>877</v>
+      </c>
+      <c r="AM20">
+        <v>868</v>
+      </c>
+      <c r="AN20">
+        <v>871</v>
+      </c>
+      <c r="AO20">
+        <v>875</v>
+      </c>
+      <c r="AP20">
+        <v>826</v>
+      </c>
+      <c r="AQ20">
+        <v>839</v>
+      </c>
+      <c r="AR20">
+        <v>831</v>
+      </c>
+      <c r="AS20">
+        <v>834</v>
+      </c>
+      <c r="AT20">
+        <v>835</v>
+      </c>
+      <c r="AU20">
+        <v>843</v>
+      </c>
+      <c r="AV20">
+        <v>840</v>
+      </c>
+      <c r="AW20">
+        <v>841</v>
+      </c>
+      <c r="AX20">
+        <v>837</v>
+      </c>
+      <c r="AY20">
+        <v>838</v>
+      </c>
+    </row>
+    <row r="21" spans="1:51" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>863</v>
+      </c>
+      <c r="B21">
+        <v>0.32323232323232326</v>
+      </c>
+      <c r="C21">
+        <v>0.47474747474747475</v>
+      </c>
+      <c r="D21">
+        <v>0.43434343434343436</v>
+      </c>
+      <c r="E21">
+        <v>0.48484848484848486</v>
+      </c>
+      <c r="F21">
+        <v>0.45454545454545453</v>
+      </c>
+      <c r="G21">
+        <v>0.30303030303030304</v>
+      </c>
+      <c r="H21">
+        <v>0.31313131313131315</v>
+      </c>
+      <c r="I21">
+        <v>0.28282828282828282</v>
+      </c>
+      <c r="J21">
+        <v>0.36363636363636365</v>
+      </c>
+      <c r="K21">
+        <v>0.38383838383838381</v>
+      </c>
+      <c r="L21">
+        <v>0.30303030303030304</v>
+      </c>
+      <c r="M21">
+        <v>0.43434343434343436</v>
+      </c>
+      <c r="N21">
+        <v>0.32323232323232326</v>
+      </c>
+      <c r="O21">
+        <v>0.48484848484848486</v>
+      </c>
+      <c r="P21">
+        <v>0.47474747474747475</v>
+      </c>
+      <c r="Q21">
+        <v>0.50505050505050508</v>
+      </c>
+      <c r="R21">
+        <v>0.36363636363636365</v>
+      </c>
+      <c r="S21">
+        <v>0.39393939393939392</v>
+      </c>
+      <c r="T21">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="U21">
+        <v>0.29292929292929293</v>
+      </c>
+      <c r="V21">
+        <v>0.28282828282828282</v>
+      </c>
+      <c r="W21">
+        <v>0.96969696969696972</v>
+      </c>
+      <c r="X21">
+        <v>0.96969696969696972</v>
+      </c>
+      <c r="Y21">
+        <v>0.97979797979797978</v>
+      </c>
+      <c r="Z21">
+        <v>0.97979797979797978</v>
+      </c>
+      <c r="AA21">
+        <v>0.32323232323232326</v>
+      </c>
+      <c r="AB21">
+        <v>0.49494949494949497</v>
+      </c>
+      <c r="AC21">
+        <v>0.45454545454545453</v>
+      </c>
+      <c r="AD21">
+        <v>0.48484848484848486</v>
+      </c>
+      <c r="AE21">
+        <v>0.48484848484848486</v>
+      </c>
+      <c r="AF21">
+        <v>0.29292929292929293</v>
+      </c>
+      <c r="AG21">
+        <v>0.46464646464646464</v>
+      </c>
+      <c r="AH21">
+        <v>0.35353535353535354</v>
+      </c>
+      <c r="AI21">
+        <v>0.41414141414141414</v>
+      </c>
+      <c r="AJ21">
+        <v>0.44444444444444442</v>
+      </c>
+      <c r="AK21">
+        <v>0.59595959595959591</v>
+      </c>
+      <c r="AL21">
+        <v>0.76767676767676762</v>
+      </c>
+      <c r="AM21">
+        <v>0.6767676767676768</v>
+      </c>
+      <c r="AN21">
+        <v>0.70707070707070707</v>
+      </c>
+      <c r="AO21">
+        <v>0.74747474747474751</v>
+      </c>
+      <c r="AP21">
+        <v>0.25252525252525254</v>
+      </c>
+      <c r="AQ21">
+        <v>0.38383838383838381</v>
+      </c>
+      <c r="AR21">
+        <v>0.30303030303030304</v>
+      </c>
+      <c r="AS21">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="AT21">
+        <v>0.34343434343434343</v>
+      </c>
+      <c r="AU21">
+        <v>0.42424242424242425</v>
+      </c>
+      <c r="AV21">
+        <v>0.39393939393939392</v>
+      </c>
+      <c r="AW21">
+        <v>0.40404040404040403</v>
+      </c>
+      <c r="AX21">
+        <v>0.36363636363636365</v>
+      </c>
+      <c r="AY21">
+        <v>0.37373737373737376</v>
+      </c>
+    </row>
+    <row r="32" spans="1:51" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>874</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>875</v>
+      </c>
+      <c r="B33" t="s">
+        <v>876</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A34">
+        <v>0</v>
+      </c>
+      <c r="B34" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A35">
+        <v>1</v>
+      </c>
+      <c r="B35" t="s">
+        <v>865</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A36">
+        <v>2</v>
+      </c>
+      <c r="B36" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A37">
+        <v>3</v>
+      </c>
+      <c r="B37" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A38">
+        <v>4</v>
+      </c>
+      <c r="B38" t="s">
+        <v>144</v>
+      </c>
+      <c r="C38" t="s">
+        <v>865</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A39">
+        <v>5</v>
+      </c>
+      <c r="B39" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A40">
+        <v>6</v>
+      </c>
+      <c r="B40" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A41">
+        <v>7</v>
+      </c>
+      <c r="B41" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A42">
+        <v>8</v>
+      </c>
+      <c r="B42" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A43">
+        <v>9</v>
+      </c>
+      <c r="B43" t="s">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
+  <conditionalFormatting sqref="B21:F21">
+    <cfRule type="colorScale" priority="10">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G21:K21">
+    <cfRule type="colorScale" priority="9">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L21:P21">
+    <cfRule type="colorScale" priority="8">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Q21:U21">
+    <cfRule type="colorScale" priority="7">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="V21:Z21">
+    <cfRule type="colorScale" priority="6">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AA21:AE21">
+    <cfRule type="colorScale" priority="5">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AF21:AJ21">
+    <cfRule type="colorScale" priority="4">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AK21:AO21">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AP21:AT21">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AU21:AY22">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
@@ -56148,7 +57466,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Added table to the results
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15460" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11700" windowHeight="16000" tabRatio="500" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="results" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5235" uniqueCount="877">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5248" uniqueCount="883">
   <si>
     <t>COLORHISTOGRAM</t>
   </si>
@@ -2640,21 +2640,6 @@
     <t>942.jpg</t>
   </si>
   <si>
-    <t>Color Histogram</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CH with Perceptual Similarity incorporated </t>
-  </si>
-  <si>
-    <t>Histogram Refinement with Color Coherence</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CH with Centering Refinement </t>
-  </si>
-  <si>
-    <t>CH with Centering Refinement and Color Coherence</t>
-  </si>
-  <si>
     <t>TOP Methods</t>
   </si>
   <si>
@@ -2662,13 +2647,61 @@
   </si>
   <si>
     <t>Method</t>
+  </si>
+  <si>
+    <t>CH</t>
+  </si>
+  <si>
+    <t>PS</t>
+  </si>
+  <si>
+    <t>CR</t>
+  </si>
+  <si>
+    <t>CV</t>
+  </si>
+  <si>
+    <t>CV + CR</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Histogram Refinement with Color Coherence </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="MS Mincho"/>
+        <charset val="128"/>
+      </rPr>
+      <t> +</t>
+    </r>
+  </si>
+  <si>
+    <t>Color Histogram with Centering Refinement and Color Coherence</t>
+  </si>
+  <si>
+    <t>Color Histogram Method</t>
+  </si>
+  <si>
+    <t>Histogram Refinement with Color Coherence and Color Histogram with Centering Refinement and Color Coherence</t>
+  </si>
+  <si>
+    <t>CH with Centering Refinement</t>
+  </si>
+  <si>
+    <t>Table 1. Image Retrieval methods with highest precision per sub class query</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="0.000"/>
+  </numFmts>
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -2697,6 +2730,12 @@
       <color theme="1"/>
       <name val="TwCenMT"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="MS Mincho"/>
+      <charset val="128"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -2706,7 +2745,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -2714,38 +2753,110 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="13">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -2787,8 +2898,13 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Method Precision</a:t>
+              <a:t>Color-Based</a:t>
             </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Image Retrieval Methods Precision and Recall</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -2923,19 +3039,19 @@
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>Color Histogram</c:v>
+                  <c:v>CH</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>CH with Perceptual Similarity incorporated </c:v>
+                  <c:v>PS</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Histogram Refinement with Color Coherence</c:v>
+                  <c:v>CV</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>CH with Centering Refinement </c:v>
+                  <c:v>CR</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>CH with Centering Refinement and Color Coherence</c:v>
+                  <c:v>CV + CR</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2944,7 +3060,7 @@
             <c:numRef>
               <c:f>Sheet1!$A$2:$E$2</c:f>
               <c:numCache>
-                <c:formatCode>0.00</c:formatCode>
+                <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>0.360606060606061</c:v>
@@ -2976,11 +3092,11 @@
         </c:dLbls>
         <c:gapWidth val="100"/>
         <c:overlap val="-24"/>
-        <c:axId val="-1614211600"/>
-        <c:axId val="-1610925936"/>
+        <c:axId val="119072608"/>
+        <c:axId val="119076416"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1614211600"/>
+        <c:axId val="119072608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3020,7 +3136,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1610925936"/>
+        <c:crossAx val="119076416"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3028,7 +3144,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1610925936"/>
+        <c:axId val="119076416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3075,7 +3191,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1614211600"/>
+        <c:crossAx val="119072608"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -54781,8 +54897,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AY43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="B43" sqref="B43"/>
+    <sheetView topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="A34" sqref="A34:B43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -57242,15 +57358,15 @@
     </row>
     <row r="32" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>874</v>
+        <v>869</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>875</v>
+        <v>870</v>
       </c>
       <c r="B33" t="s">
-        <v>876</v>
+        <v>871</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
@@ -57464,10 +57580,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="B45" sqref="B45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -57481,22 +57597,22 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>869</v>
+        <v>872</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>870</v>
+        <v>873</v>
       </c>
       <c r="C1" t="s">
-        <v>871</v>
+        <v>875</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>872</v>
+        <v>874</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>873</v>
+        <v>876</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>0.3606060606060606</v>
       </c>
@@ -57511,6 +57627,100 @@
       </c>
       <c r="E2" s="2">
         <v>0.49797979797979791</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="29" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="3" t="s">
+        <v>870</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>871</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" ht="33" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="5">
+        <v>0</v>
+      </c>
+      <c r="B30" s="6" t="s">
+        <v>877</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" ht="33" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="5">
+        <v>1</v>
+      </c>
+      <c r="B31" s="6" t="s">
+        <v>878</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" ht="33" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="5">
+        <v>2</v>
+      </c>
+      <c r="B32" s="6" t="s">
+        <v>877</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="5">
+        <v>3</v>
+      </c>
+      <c r="B33" s="6" t="s">
+        <v>879</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" ht="65" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="5">
+        <v>4</v>
+      </c>
+      <c r="B34" s="6" t="s">
+        <v>880</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="5">
+        <v>5</v>
+      </c>
+      <c r="B35" s="6" t="s">
+        <v>881</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="5">
+        <v>6</v>
+      </c>
+      <c r="B36" s="6" t="s">
+        <v>881</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="5">
+        <v>7</v>
+      </c>
+      <c r="B37" s="6" t="s">
+        <v>881</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="5">
+        <v>8</v>
+      </c>
+      <c r="B38" s="6" t="s">
+        <v>881</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="5">
+        <v>9</v>
+      </c>
+      <c r="B39" s="6" t="s">
+        <v>879</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A40" s="7" t="s">
+        <v>882</v>
       </c>
     </row>
   </sheetData>

</xml_diff>